<commit_message>
Updated test suites, cases, data files, locators
</commit_message>
<xml_diff>
--- a/Data Files/buyerInfo.xlsx
+++ b/Data Files/buyerInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasyid\Katalon Studio\SauceDemo\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3042EA65-D591-43A1-AAA9-2BE51DF93C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA7DBC0-60C7-4B21-AA43-81C898B8A9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>FirstName</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t>Rasyid</t>
+  </si>
+  <si>
+    <t>Risyad</t>
+  </si>
+  <si>
+    <t>Herry</t>
+  </si>
+  <si>
+    <t>Wijaya</t>
+  </si>
+  <si>
+    <t>Fachrie</t>
+  </si>
+  <si>
+    <t>Arithianta</t>
+  </si>
+  <si>
+    <t>Ryo</t>
+  </si>
+  <si>
+    <t>Yoshiando</t>
   </si>
 </sst>
 </file>
@@ -357,13 +378,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -387,6 +413,74 @@
         <v>12760</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>12790</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>12300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>20938</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>12760</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>12760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>